<commit_message>
Added the ability to set J and K in the special program window.
</commit_message>
<xml_diff>
--- a/src/main/resources/j_k.xlsx
+++ b/src/main/resources/j_k.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laufinsconsca\IdeaProjects\coursework-project\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D74C0D-BDE0-4ED8-A3F9-972E2612E0BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A396E48C-A1A6-4367-B73B-1C475F220592}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="-108" windowWidth="22128" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="-108" windowWidth="22128" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Неявная схема" sheetId="1" r:id="rId1"/>
@@ -76,8 +76,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -358,15 +359,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -374,7 +375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10</v>
       </c>
@@ -382,7 +383,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <f t="shared" ref="A3" si="0">A2*2</f>
         <v>20</v>
@@ -392,7 +393,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>A3*2</f>
         <v>40</v>
@@ -402,7 +403,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>A4*2</f>
         <v>80</v>
@@ -412,7 +413,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <f>A5*2</f>
         <v>160</v>
@@ -422,7 +423,7 @@
         <v>2560</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>A6*2</f>
         <v>320</v>
@@ -430,14 +431,6 @@
       <c r="B7">
         <f>B6*4</f>
         <v>10240</v>
-      </c>
-      <c r="C7">
-        <f>A7*2</f>
-        <v>640</v>
-      </c>
-      <c r="D7">
-        <f>B7*4</f>
-        <v>40960</v>
       </c>
     </row>
   </sheetData>
@@ -449,8 +442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F33EB6B-B410-42B5-9209-BF4885A19F9B}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -464,80 +457,80 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>10</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="1">
         <f t="shared" ref="A3:B4" si="0">A2*2</f>
         <v>20</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="1">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <f t="shared" ref="B4" si="1">B3*2</f>
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="1">
         <f>A4*2</f>
         <v>80</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <f>B4*2</f>
         <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <f t="shared" ref="A6:B7" si="2">A5*2</f>
+      <c r="A6" s="1">
+        <f>A5*2</f>
         <v>160</v>
       </c>
-      <c r="B6">
-        <f t="shared" si="2"/>
+      <c r="B6" s="1">
+        <f>B5*2</f>
         <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="1">
+        <f t="shared" ref="A7:B9" si="2">A6*2</f>
+        <v>320</v>
+      </c>
+      <c r="B7" s="1">
         <f t="shared" si="2"/>
         <v>320</v>
       </c>
-      <c r="B7">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
         <f t="shared" si="2"/>
-        <v>320</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <f>A7*2</f>
         <v>640</v>
       </c>
-      <c r="B8">
-        <f>B7*2</f>
+      <c r="B8" s="1">
+        <f t="shared" si="2"/>
         <v>640</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <f>A8*2</f>
+      <c r="A9" s="1">
+        <f t="shared" si="2"/>
         <v>1280</v>
       </c>
-      <c r="B9">
-        <f>B8*2</f>
+      <c r="B9" s="1">
+        <f t="shared" si="2"/>
         <v>1280</v>
       </c>
     </row>

</xml_diff>